<commit_message>
chore: Update to_df.ipynb to exclude .xlsx files and add new model configurations
</commit_message>
<xml_diff>
--- a/curve/Accuracy.xlsx
+++ b/curve/Accuracy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RetinaFace\Pytorch_Retinaface\curve\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5B7C6E-5962-49C3-A7C5-3FE4C9C828A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2701C91-6324-45E5-AF3E-61FC7223FBE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Epoch</t>
   </si>
@@ -35,6 +35,18 @@
   </si>
   <si>
     <t>mobilenet0.25_epoch10_b8_lr0.001_optAdam Validation Accuracy</t>
+  </si>
+  <si>
+    <t>mobilenet0.25_epoch10_b8_lr0.01_optAdam Train Accuracy</t>
+  </si>
+  <si>
+    <t>mobilenet0.25_epoch10_b8_lr0.01_optAdam Validation Accuracy</t>
+  </si>
+  <si>
+    <t>mobilenet0.25_epoch10_b8_lr0.1_optAdam Train Accuracy</t>
+  </si>
+  <si>
+    <t>mobilenet0.25_epoch10_b8_lr0.1_optAdam Validation Accuracy</t>
   </si>
   <si>
     <t>mobilenet0.25_epoch10_b8_lr1e-05_optAdam Train Accuracy</t>
@@ -55,22 +67,25 @@
     <t>Resnet50_epoch10_b8_lr0.001_optAdam Validation Accuracy</t>
   </si>
   <si>
+    <t>Resnet50_epoch10_b8_lr0.01_optAdam Train Accuracy</t>
+  </si>
+  <si>
+    <t>Resnet50_epoch10_b8_lr0.01_optAdam Validation Accuracy</t>
+  </si>
+  <si>
+    <t>Resnet50_epoch10_b8_lr0.1_optAdam Train Accuracy</t>
+  </si>
+  <si>
+    <t>Resnet50_epoch10_b8_lr0.1_optAdam Validation Accuracy</t>
+  </si>
+  <si>
     <t>Resnet50_epoch10_b8_lr1e-05_optAdam Train Accuracy</t>
   </si>
   <si>
     <t>Resnet50_epoch10_b8_lr1e-05_optAdam Validation Accuracy</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
+    <t>nan</t>
   </si>
 </sst>
 </file>
@@ -216,7 +231,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="C00000"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -225,45 +240,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$11</c:f>
@@ -306,7 +282,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-72D5-4776-94EF-A8F7A0B8D396}"/>
+              <c16:uniqueId val="{00000000-E6FC-4F2A-82C7-0B5C9153C28F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -327,9 +303,8 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="C00000"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -337,45 +312,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$11</c:f>
@@ -418,7 +354,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-72D5-4776-94EF-A8F7A0B8D396}"/>
+              <c16:uniqueId val="{00000001-E6FC-4F2A-82C7-0B5C9153C28F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -439,7 +375,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="FFC000"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -448,45 +384,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$D$2:$D$11</c:f>
@@ -529,7 +426,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-72D5-4776-94EF-A8F7A0B8D396}"/>
+              <c16:uniqueId val="{00000002-E6FC-4F2A-82C7-0B5C9153C28F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -550,9 +447,8 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="FFC000"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -560,45 +456,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$E$2:$E$11</c:f>
@@ -641,7 +498,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-72D5-4776-94EF-A8F7A0B8D396}"/>
+              <c16:uniqueId val="{00000003-E6FC-4F2A-82C7-0B5C9153C28F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -654,7 +511,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>mobilenet0.25_epoch10_b8_lr1e-05_optAdam Train Accuracy</c:v>
+                  <c:v>mobilenet0.25_epoch10_b8_lr0.01_optAdam Train Accuracy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -662,7 +519,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="92D050"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -671,45 +528,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$F$2:$F$11</c:f>
@@ -717,34 +535,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.0944833016306399</c:v>
+                  <c:v>2.3377375068883799</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.93740004738532401</c:v>
+                  <c:v>12.4717785448761</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.57147681018095</c:v>
+                  <c:v>14.0363203574056</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.27691029929706</c:v>
+                  <c:v>16.168634122716899</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.7902232639589902E-2</c:v>
+                  <c:v>16.8903527948363</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.6685674987539501E-2</c:v>
+                  <c:v>19.190196319547301</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.6456781989310505E-2</c:v>
+                  <c:v>20.157074302663599</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.32613763944097601</c:v>
+                  <c:v>24.132050117062999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.98748108507992205</c:v>
+                  <c:v>28.756887357343501</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.03079215871223</c:v>
+                  <c:v>29.311510026792899</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -752,7 +570,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-72D5-4776-94EF-A8F7A0B8D396}"/>
+              <c16:uniqueId val="{00000004-E6FC-4F2A-82C7-0B5C9153C28F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -765,7 +583,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>mobilenet0.25_epoch10_b8_lr1e-05_optAdam Validation Accuracy</c:v>
+                  <c:v>mobilenet0.25_epoch10_b8_lr0.01_optAdam Validation Accuracy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -773,9 +591,8 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="92D050"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
-              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -783,45 +600,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$G$2:$G$11</c:f>
@@ -829,34 +607,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.61237693912500002</c:v>
+                  <c:v>14.2677112190075</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1825206118703799</c:v>
+                  <c:v>9.9956074695269805</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.53565004597745</c:v>
+                  <c:v>17.099371638290702</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57427926161114895</c:v>
+                  <c:v>16.9140320595499</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.37732166859396399</c:v>
+                  <c:v>17.696317961673699</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.125153539476696</c:v>
+                  <c:v>18.744760030420601</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.57063236476864998</c:v>
+                  <c:v>19.016135410836601</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.83913125642083</c:v>
+                  <c:v>29.908463929881002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.13567935402348</c:v>
+                  <c:v>29.970883389630401</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.6838036997978398</c:v>
+                  <c:v>30.029247161376901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -864,7 +642,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-72D5-4776-94EF-A8F7A0B8D396}"/>
+              <c16:uniqueId val="{00000005-E6FC-4F2A-82C7-0B5C9153C28F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -877,7 +655,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Resnet50_epoch10_b8_lr0.0001_optAdam Train Accuracy</c:v>
+                  <c:v>mobilenet0.25_epoch10_b8_lr0.1_optAdam Train Accuracy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -885,7 +663,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -894,45 +674,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$H$2:$H$11</c:f>
@@ -940,34 +681,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8.5728147677317104</c:v>
+                  <c:v>2.5731899133472701E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28.0688613351155</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.219972779807399</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41.556877257982002</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45.311753898626698</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>47.021631164645299</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>49.2685303264753</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>51.654156562574599</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>51.253416786327499</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>52.286222095301902</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -975,7 +716,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-72D5-4776-94EF-A8F7A0B8D396}"/>
+              <c16:uniqueId val="{00000006-E6FC-4F2A-82C7-0B5C9153C28F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -988,7 +729,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Resnet50_epoch10_b8_lr0.0001_optAdam Validation Accuracy</c:v>
+                  <c:v>mobilenet0.25_epoch10_b8_lr0.1_optAdam Validation Accuracy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -996,9 +737,10 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
-              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1006,45 +748,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$I$2:$I$11</c:f>
@@ -1052,34 +755,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>18.468233527076901</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.778966075956198</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43.748249134661897</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42.549168603853403</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45.859306809590699</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43.510297676287998</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>47.571638012732897</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>52.451112313924902</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>51.136163200720297</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>51.451911776286103</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1087,7 +790,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-72D5-4776-94EF-A8F7A0B8D396}"/>
+              <c16:uniqueId val="{00000007-E6FC-4F2A-82C7-0B5C9153C28F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1100,7 +803,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Resnet50_epoch10_b8_lr0.001_optAdam Train Accuracy</c:v>
+                  <c:v>mobilenet0.25_epoch10_b8_lr1e-05_optAdam Train Accuracy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1108,7 +811,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="002060"/>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1117,45 +822,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$J$2:$J$11</c:f>
@@ -1163,34 +829,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.80166471570221E-2</c:v>
+                  <c:v>1.0944833016306399</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2117993982045201</c:v>
+                  <c:v>0.93740004738532401</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.5082323581137</c:v>
+                  <c:v>1.57147681018095</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.779771284031</c:v>
+                  <c:v>1.27691029929706</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22.2916844977496</c:v>
+                  <c:v>6.7902232639589902E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.252027483422701</c:v>
+                  <c:v>2.6685674987539501E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26.913245013593201</c:v>
+                  <c:v>8.6456781989310505E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34.133811194534601</c:v>
+                  <c:v>0.32613763944097601</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36.001438507815799</c:v>
+                  <c:v>0.98748108507992205</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>38.793831930747203</c:v>
+                  <c:v>2.03079215871223</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1198,7 +864,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-72D5-4776-94EF-A8F7A0B8D396}"/>
+              <c16:uniqueId val="{00000008-E6FC-4F2A-82C7-0B5C9153C28F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1211,7 +877,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Resnet50_epoch10_b8_lr0.001_optAdam Validation Accuracy</c:v>
+                  <c:v>mobilenet0.25_epoch10_b8_lr1e-05_optAdam Validation Accuracy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1219,9 +885,10 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="002060"/>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
-              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1229,45 +896,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$K$2:$K$11</c:f>
@@ -1275,34 +903,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.61237693912500002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.8986870382524792</c:v>
+                  <c:v>1.1825206118703799</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.629154458976</c:v>
+                  <c:v>1.53565004597745</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.975781088607299</c:v>
+                  <c:v>0.57427926161114895</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29.9083299482933</c:v>
+                  <c:v>0.37732166859396399</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.5206283889956</c:v>
+                  <c:v>0.125153539476696</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25.269870924933102</c:v>
+                  <c:v>0.57063236476864998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34.5595762605369</c:v>
+                  <c:v>1.83913125642083</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>37.796775021341503</c:v>
+                  <c:v>2.13567935402348</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>38.5507310506257</c:v>
+                  <c:v>3.6838036997978398</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1310,7 +938,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-72D5-4776-94EF-A8F7A0B8D396}"/>
+              <c16:uniqueId val="{00000009-E6FC-4F2A-82C7-0B5C9153C28F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1323,7 +951,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Resnet50_epoch10_b8_lr1e-05_optAdam Train Accuracy</c:v>
+                  <c:v>Resnet50_epoch10_b8_lr0.0001_optAdam Train Accuracy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1331,7 +959,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="7030A0"/>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1340,45 +970,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$L$2:$L$11</c:f>
@@ -1386,34 +977,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.42343057151042801</c:v>
+                  <c:v>8.5728147677317104</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.158385514532666</c:v>
+                  <c:v>28.0688613351155</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.55367276106030805</c:v>
+                  <c:v>36.219972779807399</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7455939026626299</c:v>
+                  <c:v>41.556877257982002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.3769521261612301</c:v>
+                  <c:v>45.311753898626698</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.04435731054373</c:v>
+                  <c:v>47.021631164645299</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.339500624093899</c:v>
+                  <c:v>49.2685303264753</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16.5805121928814</c:v>
+                  <c:v>51.654156562574599</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>19.835308142957999</c:v>
+                  <c:v>51.253416786327499</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>23.3175586495584</c:v>
+                  <c:v>52.286222095301902</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1421,7 +1012,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-72D5-4776-94EF-A8F7A0B8D396}"/>
+              <c16:uniqueId val="{0000000A-E6FC-4F2A-82C7-0B5C9153C28F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1434,7 +1025,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Resnet50_epoch10_b8_lr1e-05_optAdam Validation Accuracy</c:v>
+                  <c:v>Resnet50_epoch10_b8_lr0.0001_optAdam Validation Accuracy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1442,9 +1033,10 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="7030A0"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
-              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1452,45 +1044,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$M$2:$M$11</c:f>
@@ -1498,34 +1051,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.1924167465286</c:v>
+                  <c:v>18.468233527076901</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.33446850234569198</c:v>
+                  <c:v>25.778966075956198</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.7969354714235504</c:v>
+                  <c:v>43.748249134661897</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.3754450927043003</c:v>
+                  <c:v>42.549168603853403</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.0110371232304</c:v>
+                  <c:v>45.859306809590699</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.1625461466841802</c:v>
+                  <c:v>43.510297676287998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19.8707942432255</c:v>
+                  <c:v>47.571638012732897</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.9610179596644</c:v>
+                  <c:v>52.451112313924902</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13.6532833226132</c:v>
+                  <c:v>51.136163200720297</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22.2641318997285</c:v>
+                  <c:v>51.451911776286103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1533,7 +1086,605 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-72D5-4776-94EF-A8F7A0B8D396}"/>
+              <c16:uniqueId val="{0000000B-E6FC-4F2A-82C7-0B5C9153C28F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Resnet50_epoch10_b8_lr0.001_optAdam Train Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$2:$N$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.80166471570221E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2117993982045201</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.5082323581137</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.779771284031</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.2916844977496</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.252027483422701</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26.913245013593201</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34.133811194534601</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36.001438507815799</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38.793831930747203</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-E6FC-4F2A-82C7-0B5C9153C28F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Resnet50_epoch10_b8_lr0.001_optAdam Validation Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$2:$O$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.8986870382524792</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.629154458976</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.975781088607299</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.9083299482933</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.5206283889956</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.269870924933102</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34.5595762605369</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37.796775021341503</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38.5507310506257</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-E6FC-4F2A-82C7-0B5C9153C28F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="14"/>
+          <c:order val="14"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Resnet50_epoch10_b8_lr0.01_optAdam Train Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.5902894001616E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.7743535317619294E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2984469927954401</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.8674678088795602</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.3539905781988804</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.4158020014456598</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.505976653519699</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.250935140883101</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.6417040771492</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-E6FC-4F2A-82C7-0B5C9153C28F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="15"/>
+          <c:order val="15"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Resnet50_epoch10_b8_lr0.01_optAdam Validation Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$2:$Q$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1753419060881898</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.79195743903910998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.32834862571597</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.549220713568401</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.3272454811040202</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.0598192086561</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.850737794816601</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.3412993968932</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000F-E6FC-4F2A-82C7-0B5C9153C28F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="16"/>
+          <c:order val="16"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Resnet50_epoch10_b8_lr0.1_optAdam Train Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$2:$R$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.64121235732969895</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.24497839123565E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8452245561602598E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.9318742351028001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.89924262539073396</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1727245708823301E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.17699643159897899</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1066608362316301E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.2263624542248097E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.9069046425903</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000010-E6FC-4F2A-82C7-0B5C9153C28F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="17"/>
+          <c:order val="17"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$S$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Resnet50_epoch10_b8_lr0.1_optAdam Validation Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$S$2:$S$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.9556702728967399</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.1057051161061099E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.3945215205077703</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000011-E6FC-4F2A-82C7-0B5C9153C28F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="18"/>
+          <c:order val="18"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Resnet50_epoch10_b8_lr1e-05_optAdam Train Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$T$2:$T$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.42343057151042801</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.158385514532666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.55367276106030805</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7455939026626299</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3769521261612301</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.04435731054373</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.339500624093899</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.5805121928814</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19.835308142957999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23.3175586495584</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000012-E6FC-4F2A-82C7-0B5C9153C28F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="19"/>
+          <c:order val="19"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$U$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Resnet50_epoch10_b8_lr1e-05_optAdam Validation Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$U$2:$U$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.1924167465286</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33446850234569198</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7969354714235504</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.3754450927043003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.0110371232304</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.1625461466841802</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.8707942432255</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.9610179596644</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.6532833226132</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.2641318997285</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000013-E6FC-4F2A-82C7-0B5C9153C28F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1546,11 +1697,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="726220287"/>
-        <c:axId val="726218623"/>
+        <c:axId val="1760423840"/>
+        <c:axId val="1760425504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="726220287"/>
+        <c:axId val="1760423840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1593,7 +1744,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="726218623"/>
+        <c:crossAx val="1760425504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1601,7 +1752,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="726218623"/>
+        <c:axId val="1760425504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1652,8 +1803,8 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="726220287"/>
-        <c:crossesAt val="1"/>
+        <c:crossAx val="1760423840"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -1666,29 +1817,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:legendEntry>
-        <c:idx val="3"/>
-        <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-      </c:legendEntry>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2315,23 +2443,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>183251</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>155504</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>289891</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>62119</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76C9BA00-606E-40C0-BCE0-2D96DBF50820}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B72B09C-E41F-4703-B0B8-330739029F70}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2637,18 +2765,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="8.140625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2688,8 +2813,32 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2706,31 +2855,55 @@
         <v>12.155477515828499</v>
       </c>
       <c r="F2" s="1">
+        <v>2.3377375068883799</v>
+      </c>
+      <c r="G2" s="1">
+        <v>14.2677112190075</v>
+      </c>
+      <c r="H2" s="1">
+        <v>2.5731899133472701E-2</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="1">
         <v>1.0944833016306399</v>
       </c>
-      <c r="G2" s="1">
+      <c r="K2" s="1">
         <v>0.61237693912500002</v>
       </c>
-      <c r="H2" s="1">
+      <c r="L2" s="1">
         <v>8.5728147677317104</v>
       </c>
-      <c r="I2" s="1">
+      <c r="M2" s="1">
         <v>18.468233527076901</v>
       </c>
-      <c r="J2" s="1">
+      <c r="N2" s="1">
         <v>1.80166471570221E-2</v>
       </c>
-      <c r="K2" s="1">
+      <c r="O2" s="1">
         <v>0</v>
       </c>
-      <c r="L2" s="1">
+      <c r="P2" s="1">
+        <v>2.5902894001616E-3</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0.64121235732969895</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1">
         <v>0.42343057151042801</v>
       </c>
-      <c r="M2" s="1">
+      <c r="U2" s="1">
         <v>1.1924167465286</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2747,31 +2920,55 @@
         <v>24.503143663778399</v>
       </c>
       <c r="F3" s="1">
+        <v>12.4717785448761</v>
+      </c>
+      <c r="G3" s="1">
+        <v>9.9956074695269805</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
         <v>0.93740004738532401</v>
       </c>
-      <c r="G3" s="1">
+      <c r="K3" s="1">
         <v>1.1825206118703799</v>
       </c>
-      <c r="H3" s="1">
+      <c r="L3" s="1">
         <v>28.0688613351155</v>
       </c>
-      <c r="I3" s="1">
+      <c r="M3" s="1">
         <v>25.778966075956198</v>
       </c>
-      <c r="J3" s="1">
+      <c r="N3" s="1">
         <v>2.2117993982045201</v>
       </c>
-      <c r="K3" s="1">
+      <c r="O3" s="1">
         <v>9.8986870382524792</v>
       </c>
-      <c r="L3" s="1">
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1">
+        <v>8.24497839123565E-4</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T3" s="1">
         <v>0.158385514532666</v>
       </c>
-      <c r="M3" s="1">
+      <c r="U3" s="1">
         <v>0.33446850234569198</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2788,31 +2985,55 @@
         <v>27.053781332615799</v>
       </c>
       <c r="F4" s="1">
+        <v>14.0363203574056</v>
+      </c>
+      <c r="G4" s="1">
+        <v>17.099371638290702</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
         <v>1.57147681018095</v>
       </c>
-      <c r="G4" s="1">
+      <c r="K4" s="1">
         <v>1.53565004597745</v>
       </c>
-      <c r="H4" s="1">
+      <c r="L4" s="1">
         <v>36.219972779807399</v>
       </c>
-      <c r="I4" s="1">
+      <c r="M4" s="1">
         <v>43.748249134661897</v>
       </c>
-      <c r="J4" s="1">
+      <c r="N4" s="1">
         <v>11.5082323581137</v>
       </c>
-      <c r="K4" s="1">
+      <c r="O4" s="1">
         <v>15.629154458976</v>
       </c>
-      <c r="L4" s="1">
+      <c r="P4" s="1">
+        <v>7.7743535317619294E-2</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>3.1753419060881898</v>
+      </c>
+      <c r="R4" s="1">
+        <v>6.8452245561602598E-3</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1">
         <v>0.55367276106030805</v>
       </c>
-      <c r="M4" s="1">
+      <c r="U4" s="1">
         <v>5.7969354714235504</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2829,31 +3050,55 @@
         <v>28.987131675202001</v>
       </c>
       <c r="F5" s="1">
+        <v>16.168634122716899</v>
+      </c>
+      <c r="G5" s="1">
+        <v>16.9140320595499</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
         <v>1.27691029929706</v>
       </c>
-      <c r="G5" s="1">
+      <c r="K5" s="1">
         <v>0.57427926161114895</v>
       </c>
-      <c r="H5" s="1">
+      <c r="L5" s="1">
         <v>41.556877257982002</v>
       </c>
-      <c r="I5" s="1">
+      <c r="M5" s="1">
         <v>42.549168603853403</v>
       </c>
-      <c r="J5" s="1">
+      <c r="N5" s="1">
         <v>16.779771284031</v>
       </c>
-      <c r="K5" s="1">
+      <c r="O5" s="1">
         <v>19.975781088607299</v>
       </c>
-      <c r="L5" s="1">
+      <c r="P5" s="1">
+        <v>1.2984469927954401</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0.79195743903910998</v>
+      </c>
+      <c r="R5" s="1">
+        <v>6.9318742351028001E-2</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
         <v>1.7455939026626299</v>
       </c>
-      <c r="M5" s="1">
+      <c r="U5" s="1">
         <v>6.3754450927043003</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2870,31 +3115,55 @@
         <v>37.461600273911202</v>
       </c>
       <c r="F6" s="1">
+        <v>16.8903527948363</v>
+      </c>
+      <c r="G6" s="1">
+        <v>17.696317961673699</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
         <v>6.7902232639589902E-2</v>
       </c>
-      <c r="G6" s="1">
+      <c r="K6" s="1">
         <v>0.37732166859396399</v>
       </c>
-      <c r="H6" s="1">
+      <c r="L6" s="1">
         <v>45.311753898626698</v>
       </c>
-      <c r="I6" s="1">
+      <c r="M6" s="1">
         <v>45.859306809590699</v>
       </c>
-      <c r="J6" s="1">
+      <c r="N6" s="1">
         <v>22.2916844977496</v>
       </c>
-      <c r="K6" s="1">
+      <c r="O6" s="1">
         <v>29.9083299482933</v>
       </c>
-      <c r="L6" s="1">
+      <c r="P6" s="1">
+        <v>3.8674678088795602</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>1.32834862571597</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0.89924262539073396</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1">
         <v>3.3769521261612301</v>
       </c>
-      <c r="M6" s="1">
+      <c r="U6" s="1">
         <v>11.0110371232304</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2911,31 +3180,55 @@
         <v>37.353114490753697</v>
       </c>
       <c r="F7" s="1">
+        <v>19.190196319547301</v>
+      </c>
+      <c r="G7" s="1">
+        <v>18.744760030420601</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
         <v>2.6685674987539501E-2</v>
       </c>
-      <c r="G7" s="1">
+      <c r="K7" s="1">
         <v>0.125153539476696</v>
       </c>
-      <c r="H7" s="1">
+      <c r="L7" s="1">
         <v>47.021631164645299</v>
       </c>
-      <c r="I7" s="1">
+      <c r="M7" s="1">
         <v>43.510297676287998</v>
       </c>
-      <c r="J7" s="1">
+      <c r="N7" s="1">
         <v>25.252027483422701</v>
       </c>
-      <c r="K7" s="1">
+      <c r="O7" s="1">
         <v>22.5206283889956</v>
       </c>
-      <c r="L7" s="1">
+      <c r="P7" s="1">
+        <v>5.3539905781988804</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>10.549220713568401</v>
+      </c>
+      <c r="R7" s="1">
+        <v>2.1727245708823301E-2</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1">
         <v>6.04435731054373</v>
       </c>
-      <c r="M7" s="1">
+      <c r="U7" s="1">
         <v>9.1625461466841802</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2952,31 +3245,55 @@
         <v>36.494410965418098</v>
       </c>
       <c r="F8" s="1">
+        <v>20.157074302663599</v>
+      </c>
+      <c r="G8" s="1">
+        <v>19.016135410836601</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
         <v>8.6456781989310505E-2</v>
       </c>
-      <c r="G8" s="1">
+      <c r="K8" s="1">
         <v>0.57063236476864998</v>
       </c>
-      <c r="H8" s="1">
+      <c r="L8" s="1">
         <v>49.2685303264753</v>
       </c>
-      <c r="I8" s="1">
+      <c r="M8" s="1">
         <v>47.571638012732897</v>
       </c>
-      <c r="J8" s="1">
+      <c r="N8" s="1">
         <v>26.913245013593201</v>
       </c>
-      <c r="K8" s="1">
+      <c r="O8" s="1">
         <v>25.269870924933102</v>
       </c>
-      <c r="L8" s="1">
+      <c r="P8" s="1">
+        <v>7.4158020014456598</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>6.3272454811040202</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0.17699643159897899</v>
+      </c>
+      <c r="S8" s="1">
+        <v>3.9556702728967399</v>
+      </c>
+      <c r="T8" s="1">
         <v>10.339500624093899</v>
       </c>
-      <c r="M8" s="1">
+      <c r="U8" s="1">
         <v>19.8707942432255</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2993,31 +3310,55 @@
         <v>44.519702802718697</v>
       </c>
       <c r="F9" s="1">
+        <v>24.132050117062999</v>
+      </c>
+      <c r="G9" s="1">
+        <v>29.908463929881002</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
         <v>0.32613763944097601</v>
       </c>
-      <c r="G9" s="1">
+      <c r="K9" s="1">
         <v>1.83913125642083</v>
       </c>
-      <c r="H9" s="1">
+      <c r="L9" s="1">
         <v>51.654156562574599</v>
       </c>
-      <c r="I9" s="1">
+      <c r="M9" s="1">
         <v>52.451112313924902</v>
       </c>
-      <c r="J9" s="1">
+      <c r="N9" s="1">
         <v>34.133811194534601</v>
       </c>
-      <c r="K9" s="1">
+      <c r="O9" s="1">
         <v>34.5595762605369</v>
       </c>
-      <c r="L9" s="1">
+      <c r="P9" s="1">
+        <v>11.505976653519699</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>14.0598192086561</v>
+      </c>
+      <c r="R9" s="1">
+        <v>1.1066608362316301E-2</v>
+      </c>
+      <c r="S9" s="1">
+        <v>0</v>
+      </c>
+      <c r="T9" s="1">
         <v>16.5805121928814</v>
       </c>
-      <c r="M9" s="1">
+      <c r="U9" s="1">
         <v>14.9610179596644</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3034,31 +3375,55 @@
         <v>43.871012136959401</v>
       </c>
       <c r="F10" s="1">
+        <v>28.756887357343501</v>
+      </c>
+      <c r="G10" s="1">
+        <v>29.970883389630401</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
         <v>0.98748108507992205</v>
       </c>
-      <c r="G10" s="1">
+      <c r="K10" s="1">
         <v>2.13567935402348</v>
       </c>
-      <c r="H10" s="1">
+      <c r="L10" s="1">
         <v>51.253416786327499</v>
       </c>
-      <c r="I10" s="1">
+      <c r="M10" s="1">
         <v>51.136163200720297</v>
       </c>
-      <c r="J10" s="1">
+      <c r="N10" s="1">
         <v>36.001438507815799</v>
       </c>
-      <c r="K10" s="1">
+      <c r="O10" s="1">
         <v>37.796775021341503</v>
       </c>
-      <c r="L10" s="1">
+      <c r="P10" s="1">
+        <v>13.250935140883101</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>14.850737794816601</v>
+      </c>
+      <c r="R10" s="1">
+        <v>7.2263624542248097E-3</v>
+      </c>
+      <c r="S10" s="1">
+        <v>2.1057051161061099E-2</v>
+      </c>
+      <c r="T10" s="1">
         <v>19.835308142957999</v>
       </c>
-      <c r="M10" s="1">
+      <c r="U10" s="1">
         <v>13.6532833226132</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3075,27 +3440,51 @@
         <v>48.698255497499403</v>
       </c>
       <c r="F11" s="1">
+        <v>29.311510026792899</v>
+      </c>
+      <c r="G11" s="1">
+        <v>30.029247161376901</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
         <v>2.03079215871223</v>
       </c>
-      <c r="G11" s="1">
+      <c r="K11" s="1">
         <v>3.6838036997978398</v>
       </c>
-      <c r="H11" s="1">
+      <c r="L11" s="1">
         <v>52.286222095301902</v>
       </c>
-      <c r="I11" s="1">
+      <c r="M11" s="1">
         <v>51.451911776286103</v>
       </c>
-      <c r="J11" s="1">
+      <c r="N11" s="1">
         <v>38.793831930747203</v>
       </c>
-      <c r="K11" s="1">
+      <c r="O11" s="1">
         <v>38.5507310506257</v>
       </c>
-      <c r="L11" s="1">
+      <c r="P11" s="1">
+        <v>15.6417040771492</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>15.3412993968932</v>
+      </c>
+      <c r="R11" s="1">
+        <v>2.9069046425903</v>
+      </c>
+      <c r="S11" s="1">
+        <v>5.3945215205077703</v>
+      </c>
+      <c r="T11" s="1">
         <v>23.3175586495584</v>
       </c>
-      <c r="M11" s="1">
+      <c r="U11" s="1">
         <v>22.2641318997285</v>
       </c>
     </row>

</xml_diff>